<commit_message>
refactor: Organizar seções do código e renomear comentários para melhor legibilidade
</commit_message>
<xml_diff>
--- a/export/Registros_11-2025.xlsx
+++ b/export/Registros_11-2025.xlsx
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Resumo'!$A$1:$C$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Guilherme'!$A$1:$G$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Taissa'!$A$1:$G$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Taissa'!$A$1:$G$3</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C3" s="3" t="n">
-        <v>0.05416666666666667</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -654,7 +654,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -712,121 +712,43 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>03/11/2025</t>
+          <t>05/11/2025</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Seg</t>
+          <t>Qua</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>09:34</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
-        <is>
-          <t>09:58</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>10:01</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>10:16</t>
-        </is>
-      </c>
+          <t>23:42</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr"/>
+      <c r="E2" s="2" t="inlineStr"/>
+      <c r="F2" s="2" t="inlineStr"/>
       <c r="G2" s="4" t="n">
-        <v>0.02708333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>04/11/2025</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Ter</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>09:03</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>09:05</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>09:14</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr"/>
-      <c r="G3" s="4" t="n">
+      <c r="A3" s="5" t="inlineStr"/>
+      <c r="B3" s="5" t="inlineStr"/>
+      <c r="C3" s="5" t="inlineStr"/>
+      <c r="D3" s="5" t="inlineStr"/>
+      <c r="E3" s="6" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr"/>
+      <c r="G3" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>05/11/2025</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Qua</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>09:34</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>09:58</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>10:01</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>10:16</t>
-        </is>
-      </c>
-      <c r="G4" s="4" t="n">
-        <v>0.02708333333333333</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="inlineStr"/>
-      <c r="B5" s="5" t="inlineStr"/>
-      <c r="C5" s="5" t="inlineStr"/>
-      <c r="D5" s="5" t="inlineStr"/>
-      <c r="E5" s="6" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="F5" s="5" t="inlineStr"/>
-      <c r="G5" s="7" t="n">
-        <v>0.05416666666666667</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G5"/>
+  <autoFilter ref="A1:G3"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>